<commit_message>
Added just a literal shit-ton of stuff. God help me.
</commit_message>
<xml_diff>
--- a/EventManager/Notes/DBTables.xlsx
+++ b/EventManager/Notes/DBTables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\defaultpc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\defaultpc\Documents\visual studio 2015\Projects\EventManager\EventManager\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="171">
   <si>
     <t>Field</t>
   </si>
@@ -345,13 +345,234 @@
   </si>
   <si>
     <t>NOTES</t>
+  </si>
+  <si>
+    <t>EventID</t>
+  </si>
+  <si>
+    <t>Identity(1,1)</t>
+  </si>
+  <si>
+    <t>Primary Key for entity</t>
+  </si>
+  <si>
+    <t>EventName</t>
+  </si>
+  <si>
+    <t>100 Character Limit</t>
+  </si>
+  <si>
+    <t>Display Name for Event</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>SmallDateTime</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Start Date/Time for Event</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>End Date/Time for Event</t>
+  </si>
+  <si>
+    <t>Cannot be &lt; StartTime, Enforced by DB CONSTRAINT</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Display Notes for Event</t>
+  </si>
+  <si>
+    <t>MaxStaff</t>
+  </si>
+  <si>
+    <t>Not Null</t>
+  </si>
+  <si>
+    <t>300 Character Limit, Nullable</t>
+  </si>
+  <si>
+    <t>Not Null, &gt;= MinStaff</t>
+  </si>
+  <si>
+    <t>Maximum Staffing For event</t>
+  </si>
+  <si>
+    <t>MinStaff</t>
+  </si>
+  <si>
+    <t>&gt; 0</t>
+  </si>
+  <si>
+    <t>Minimum Staffing For Event</t>
+  </si>
+  <si>
+    <t>FundCenter</t>
+  </si>
+  <si>
+    <t>25 character limit</t>
+  </si>
+  <si>
+    <t>FundCenter for Event</t>
+  </si>
+  <si>
+    <t>EnteredBy</t>
+  </si>
+  <si>
+    <t>UserID of Event Creator</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
+  </si>
+  <si>
+    <t>Date/Time Event was added to DB</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>IDNumber</t>
+  </si>
+  <si>
+    <t>PayrollID</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>Database UserID, PK for Entity</t>
+  </si>
+  <si>
+    <t>Int between 1-n (mapped to Police Rank</t>
+  </si>
+  <si>
+    <t>User's Police Rank</t>
+  </si>
+  <si>
+    <t>User's First Name</t>
+  </si>
+  <si>
+    <t>User's Last Name</t>
+  </si>
+  <si>
+    <t>50 character limit</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>User's Police ID Number</t>
+  </si>
+  <si>
+    <t>20 character limit?</t>
+  </si>
+  <si>
+    <t>320 Character limit (SMTP Standard)</t>
+  </si>
+  <si>
+    <r>
+      <t>User's Email address -</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> validate? Limit to work email?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>User's Payroll ID -</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Should this be a number?</t>
+    </r>
+  </si>
+  <si>
+    <t>10 character Max, no non-numbers?</t>
+  </si>
+  <si>
+    <t>client regex validation, server algorithm to extract numbers</t>
+  </si>
+  <si>
+    <t>not null (Validate on client or server)</t>
+  </si>
+  <si>
+    <t>RegisteredDate</t>
+  </si>
+  <si>
+    <t>not null</t>
+  </si>
+  <si>
+    <t>Date User Registered (Until linked to External Admin DB; when linked, date of first Event Registration)</t>
+  </si>
+  <si>
+    <t>RegistrationID</t>
+  </si>
+  <si>
+    <t>PK for Registration Entity</t>
+  </si>
+  <si>
+    <t>FK to User Table</t>
+  </si>
+  <si>
+    <t>FK to Events Table</t>
+  </si>
+  <si>
+    <t>TimeStamp</t>
+  </si>
+  <si>
+    <t>CONSTRAINT FK_UserID FOREIGN KEY REFERENCES Users(UserID)</t>
+  </si>
+  <si>
+    <t>CONSTRAINT FK_EventID FOREIGN KEY REFERENCES Events(EventID)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Maps to Registration Statuses (Created, Confirmed, Declined, etc?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +592,14 @@
       <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -681,41 +910,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF444444"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDDDDDD"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -958,6 +1152,41 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF444444"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -972,15 +1201,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{899E9B34-67CA-4CC8-98A6-D36986FADEAB}" name="DataTypes" displayName="DataTypes" ref="A1:F36" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{899E9B34-67CA-4CC8-98A6-D36986FADEAB}" name="DataTypes" displayName="DataTypes" ref="A1:F36" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A1:F36" xr:uid="{D35A9181-6AB1-42BA-AD5F-75FAF0D8EE89}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{62FC9488-0ABE-41BF-AB81-270159E61080}" name="SQL Server Data Types" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{DE0D03F9-43B5-4042-91FA-8D417412322A}" name="MIN" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{46AAEEEB-38A8-4AC9-AAC5-569DFCF269B1}" name="MAX" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{33671695-DBDF-4BDE-9FE8-94372C278149}" name="STORAGE" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E1C8D0B2-A317-478F-AA4E-3CF648002881}" name="TYPE" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{738BDEE1-BA43-4A1C-9023-7E7216EAA723}" name="NOTES" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{62FC9488-0ABE-41BF-AB81-270159E61080}" name="SQL Server Data Types" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{DE0D03F9-43B5-4042-91FA-8D417412322A}" name="MIN" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{46AAEEEB-38A8-4AC9-AAC5-569DFCF269B1}" name="MAX" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{33671695-DBDF-4BDE-9FE8-94372C278149}" name="STORAGE" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E1C8D0B2-A317-478F-AA4E-3CF648002881}" name="TYPE" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{738BDEE1-BA43-4A1C-9023-7E7216EAA723}" name="NOTES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1286,14 +1515,14 @@
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101:XFD1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="161.140625" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -1312,16 +1541,146 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+    </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25"/>
@@ -1433,14 +1792,14 @@
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="161.140625" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -1459,15 +1818,132 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+    </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25"/>
@@ -1560,6 +2036,7 @@
     <row r="100" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1580,14 +2057,14 @@
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" customWidth="1"/>
     <col min="4" max="4" width="161.140625" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -1606,11 +2083,73 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
+        <v>170</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25"/>

</xml_diff>